<commit_message>
gitgignore delete, possible fix
</commit_message>
<xml_diff>
--- a/SCHRACK_bom.xlsx
+++ b/SCHRACK_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\SchrackProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BFC216-4A77-4805-A7F9-2F5ACC34BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ADE36F-8611-47CC-B981-FFFF4A3714C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sumecBOM" sheetId="1" r:id="rId1"/>
@@ -33,65 +33,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Designator</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Reserve</t>
-  </si>
-  <si>
-    <t>Datasheet says it 0.6-7V output, desc.6-7V</t>
-  </si>
-  <si>
     <t>NMOS</t>
   </si>
   <si>
     <t>MAX7219</t>
   </si>
   <si>
-    <t>SOIC-24W_7.5x15.4mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>MEM2067-02-180-00-A_REVB</t>
   </si>
   <si>
     <t>MICRO_SD_CARD</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
     <t>LDD080BUE-101A</t>
   </si>
   <si>
     <t>LDD080BUE-101A_made_by_bismarx</t>
   </si>
   <si>
-    <t>U2,U4</t>
-  </si>
-  <si>
     <t>LTD080BUE-103A</t>
   </si>
   <si>
@@ -104,10 +74,19 @@
     <t>BUZZER_CUI_CPT</t>
   </si>
   <si>
-    <t>BZ1</t>
-  </si>
-  <si>
     <t>BUZZER Piezo mouser</t>
+  </si>
+  <si>
+    <t>LED MAX7219</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>DIP-24</t>
   </si>
 </sst>
 </file>
@@ -291,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,18 +470,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -510,12 +477,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,19 +665,13 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
@@ -732,16 +687,20 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1122,561 +1081,478 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.1796875" customWidth="1"/>
-    <col min="3" max="3" width="50.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="55" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" customWidth="1"/>
-    <col min="7" max="7" width="23.81640625" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="34.54296875" customWidth="1"/>
-    <col min="10" max="10" width="36.81640625" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="1"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="1"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="E6" s="1">
+        <v>38</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="8"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="8"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
+      <c r="F22" s="6"/>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="8"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="11"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="8"/>
+      <c r="F33" s="6"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="8"/>
+      <c r="F34" s="6"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
       <c r="B36" s="1"/>
-      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="8"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="1"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="1"/>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="1"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="1"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="16"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="BUZZER Piezo" xr:uid="{46ADD8D9-25A0-4066-83EF-C2C596F5E0DA}"/>
+    <hyperlink ref="D2" r:id="rId1" display="BUZZER Piezo" xr:uid="{46ADD8D9-25A0-4066-83EF-C2C596F5E0DA}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{1E4A80B1-A1ED-4971-B110-C4D2EC9BDF2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bom final, schematic updates
</commit_message>
<xml_diff>
--- a/SCHRACK_bom.xlsx
+++ b/SCHRACK_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\SchrackProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ADE36F-8611-47CC-B981-FFFF4A3714C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5000D2-2FC2-4255-B253-86811DC27D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sumecBOM" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Footprint</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Link</t>
   </si>
@@ -44,49 +41,124 @@
     <t>Value</t>
   </si>
   <si>
-    <t>NMOS</t>
-  </si>
-  <si>
-    <t>MAX7219</t>
-  </si>
-  <si>
-    <t>MEM2067-02-180-00-A_REVB</t>
-  </si>
-  <si>
-    <t>MICRO_SD_CARD</t>
-  </si>
-  <si>
-    <t>LDD080BUE-101A</t>
-  </si>
-  <si>
-    <t>LDD080BUE-101A_made_by_bismarx</t>
-  </si>
-  <si>
-    <t>LTD080BUE-103A</t>
-  </si>
-  <si>
-    <t>LTD080BUE-103A_made_by_bismarx</t>
-  </si>
-  <si>
-    <t>Buzzer</t>
-  </si>
-  <si>
-    <t>BUZZER_CUI_CPT</t>
-  </si>
-  <si>
-    <t>BUZZER Piezo mouser</t>
-  </si>
-  <si>
-    <t>LED MAX7219</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>DIP-24</t>
+    <t>LED MAX7219 LASKAKIT</t>
+  </si>
+  <si>
+    <t>CONTACT 1Z SCHRACK</t>
+  </si>
+  <si>
+    <t>CONNECTING PART SCHRACK</t>
+  </si>
+  <si>
+    <t>ROTARY SWITCH SCHRACK</t>
+  </si>
+  <si>
+    <t>MAIN PWR SWITCH SCHRACK</t>
+  </si>
+  <si>
+    <t>2DIGIT 0.8IN TME</t>
+  </si>
+  <si>
+    <t>3DIGIT 0.8IN TME</t>
+  </si>
+  <si>
+    <t>2DIGIT GME</t>
+  </si>
+  <si>
+    <t>3DIGIT GME</t>
+  </si>
+  <si>
+    <t>TACT. SWITCH SCHRACK</t>
+  </si>
+  <si>
+    <t>74HC595N LASKAKIT</t>
+  </si>
+  <si>
+    <t>PASSIVE BUZZER</t>
+  </si>
+  <si>
+    <t>SD CARD</t>
+  </si>
+  <si>
+    <t>MAX7219 - DRIVER</t>
+  </si>
+  <si>
+    <t>LTD080BUE-103A -7SEG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDD080BUE-101A -7SEG </t>
+  </si>
+  <si>
+    <t>MULTICLOCK SWITCH</t>
+  </si>
+  <si>
+    <t>BUTTON CONTACT</t>
+  </si>
+  <si>
+    <t>PLASTIC CONNECTING PART</t>
+  </si>
+  <si>
+    <t>POWER SWITCH</t>
+  </si>
+  <si>
+    <t>TACTILE SWITCH</t>
+  </si>
+  <si>
+    <t>B/W DOUBLE SWITCH</t>
+  </si>
+  <si>
+    <t>74HC595N - SHIFT REG.</t>
+  </si>
+  <si>
+    <t>B/W DOUBLE SWITCH SCHRACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT-A512RD -7SEG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD-A544RD -7SEG </t>
+  </si>
+  <si>
+    <t>SD CARD MODULE LASKAKIT</t>
+  </si>
+  <si>
+    <t>BUZZER LASKAKIT</t>
+  </si>
+  <si>
+    <t>ESP32</t>
+  </si>
+  <si>
+    <t>ESP32 - MCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRIVER </t>
+  </si>
+  <si>
+    <t>JUMPER WIRES YURI</t>
+  </si>
+  <si>
+    <t>JUMPER WIRES YAOI</t>
+  </si>
+  <si>
+    <t>JUMPER WIRES STRAIGHT</t>
+  </si>
+  <si>
+    <t>Cost total</t>
+  </si>
+  <si>
+    <t>LIGHTSWITCH SCHRACK</t>
+  </si>
+  <si>
+    <t>LIGHTSWITCH</t>
+  </si>
+  <si>
+    <t>JUMPERS</t>
   </si>
 </sst>
 </file>
@@ -270,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,12 +520,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -657,27 +723,24 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
@@ -693,14 +756,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1081,449 +1146,635 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.140625" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
     <col min="9" max="9" width="34.5703125" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="14"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="6"/>
+      <c r="A2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>SUM(C2*D2)</f>
+        <v>116</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="1"/>
-      <c r="H3" s="16"/>
+      <c r="C3" s="1">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>SUM(C3*D3)</f>
+        <v>92</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="1"/>
-      <c r="H4" s="16"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>198</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E4:E26" si="0">SUM(C5*D5)</f>
+        <v>396</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>300</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>84</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="1"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C13" s="1">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1">
-        <v>38</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="13"/>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="13"/>
+      <c r="A14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>290</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="13"/>
+      <c r="A15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1">
+        <v>121</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1">
+        <v>355</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>355</v>
+      </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="13"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="13"/>
+      <c r="A17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1">
+        <v>67</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="13"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="13"/>
+      <c r="A19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>41</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="13"/>
+      <c r="A20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
+        <v>28</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="6"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="1"/>
+      <c r="F21" s="5"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="6"/>
-      <c r="H22" s="13"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1">
+        <v>268</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>268</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="13"/>
+      <c r="A23" s="1"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="13"/>
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="13"/>
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="13"/>
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="A28" s="1"/>
+      <c r="E28" s="15">
+        <f>SUM(E2:E27)</f>
+        <v>3019</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="13"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="11"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="16"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="6"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="16"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="6"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="16"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="16"/>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="6"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="16"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
+      <c r="A37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="16"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="16"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="16"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="16"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="16"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G42" s="1"/>
-      <c r="H42" s="16"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G43" s="1"/>
-      <c r="H43" s="16"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G44" s="1"/>
-      <c r="H44" s="16"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G45" s="1"/>
-      <c r="H45" s="16"/>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
-      <c r="H46" s="16"/>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="16"/>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="16"/>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="1"/>
+      <c r="A49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="16"/>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="1"/>
+      <c r="A50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="16"/>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="16"/>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="1"/>
+      <c r="A52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="16"/>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="16"/>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="16"/>
+      <c r="H54" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
@@ -1532,27 +1783,42 @@
       <c r="F57" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
+    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
+    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E78" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="BUZZER Piezo" xr:uid="{46ADD8D9-25A0-4066-83EF-C2C596F5E0DA}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{1E4A80B1-A1ED-4971-B110-C4D2EC9BDF2D}"/>
+    <hyperlink ref="B8" r:id="rId1" display="LED MAX7219" xr:uid="{1E4A80B1-A1ED-4971-B110-C4D2EC9BDF2D}"/>
+    <hyperlink ref="B11" r:id="rId2" display="SCHRACK ROTARY SWITCH" xr:uid="{C4DF7C7D-DDB8-45BF-A437-6B583CFD7719}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{2E93ED3C-C6C4-4DB8-9085-AB7DC46E1AB7}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{E32D0610-4C22-4143-96D4-42FE9407CDB8}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{83F11D3E-8A8B-4FEB-B3D4-42A68E9E9355}"/>
+    <hyperlink ref="B3" r:id="rId6" display="2DIGIT 0.8IN" xr:uid="{580D8A90-A525-4103-80BC-86692308D035}"/>
+    <hyperlink ref="B2" r:id="rId7" display="3DIGIT 0.8IN" xr:uid="{F3A0F711-4E3D-437D-B6B1-08FEB77FF404}"/>
+    <hyperlink ref="B20" r:id="rId8" xr:uid="{D00301B1-351D-4B39-A492-6C9989CEBCC0}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{3CD4033C-9B3A-4318-9D64-ACE96F523159}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{C37A50F1-209C-4A5D-A411-0A456C588DD1}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{C12FBC33-BE35-4D16-A3DE-C0D5DD8DAB8D}"/>
+    <hyperlink ref="B16" r:id="rId12" display="B/W DOUBLE SWITCH" xr:uid="{C90E987D-AD3A-4993-9BF7-652E256C06B3}"/>
+    <hyperlink ref="B7" r:id="rId13" display="SD CARD MODULE" xr:uid="{00BC3802-F8D1-45E4-9144-911623178974}"/>
+    <hyperlink ref="B6" r:id="rId14" xr:uid="{074DFFA5-B78D-49EA-8698-C94E992C0CE2}"/>
+    <hyperlink ref="B5" r:id="rId15" location="relatedFiles" xr:uid="{115571BD-5AA3-42A8-A209-B76666A562D6}"/>
+    <hyperlink ref="B22" r:id="rId16" xr:uid="{D06EEAAB-F557-458E-A548-9BBAD34798FD}"/>
+    <hyperlink ref="B24" r:id="rId17" xr:uid="{487581BC-3942-40B1-9A68-4FCD1588123D}"/>
+    <hyperlink ref="B25" r:id="rId18" xr:uid="{721B5926-F035-438B-B5B6-1DA9415413DF}"/>
+    <hyperlink ref="B26" r:id="rId19" display="JUMPER WIRES STRAIGT" xr:uid="{AEFDAEF5-2992-43DD-8C63-EB43B385D8BA}"/>
+    <hyperlink ref="B17" r:id="rId20" xr:uid="{15437A6C-D298-45C0-863D-AE58A8E10838}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
totally didnt add gay wires to the BOM
</commit_message>
<xml_diff>
--- a/SCHRACK_bom.xlsx
+++ b/SCHRACK_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\SchrackProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5000D2-2FC2-4255-B253-86811DC27D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF91609-EF41-405F-89F2-152A44D9A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Link</t>
   </si>
@@ -131,24 +131,9 @@
     <t>BUZZER LASKAKIT</t>
   </si>
   <si>
-    <t>ESP32</t>
-  </si>
-  <si>
     <t>ESP32 - MCU</t>
   </si>
   <si>
-    <t xml:space="preserve">DRIVER </t>
-  </si>
-  <si>
-    <t>JUMPER WIRES YURI</t>
-  </si>
-  <si>
-    <t>JUMPER WIRES YAOI</t>
-  </si>
-  <si>
-    <t>JUMPER WIRES STRAIGHT</t>
-  </si>
-  <si>
     <t>Cost total</t>
   </si>
   <si>
@@ -159,6 +144,24 @@
   </si>
   <si>
     <t>JUMPERS</t>
+  </si>
+  <si>
+    <t>ESP32 LASKAKIT</t>
+  </si>
+  <si>
+    <t>JUMPER WIRES YURI LASKAKIT</t>
+  </si>
+  <si>
+    <t>JUMPER WIRES YAOI LASKAKIT</t>
+  </si>
+  <si>
+    <t>JUMPER WIRES STRAIGHT LASKAKIT</t>
+  </si>
+  <si>
+    <t>DRIVER LASKAKIT</t>
+  </si>
+  <si>
+    <t>DRIVER</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,8 +768,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1147,13 +1153,13 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -1165,7 +1171,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -1178,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H1" s="12"/>
     </row>
@@ -1225,11 +1231,11 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
+      <c r="A5" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1">
         <v>198</v>
@@ -1238,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E4:E26" si="0">SUM(C5*D5)</f>
+        <f t="shared" ref="E5:E26" si="0">SUM(C5*D5)</f>
         <v>396</v>
       </c>
       <c r="H5" s="1"/>
@@ -1324,26 +1330,41 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>SUM(C10*D10)</f>
+        <v>52</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
-        <v>300</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>SUM(C11*D11)</f>
+        <v>52</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="8"/>
@@ -1352,100 +1373,84 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>252</v>
+        <f>SUM(C12*D12)</f>
+        <v>52</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>114</v>
+        <f>SUM(C13*D13)</f>
+        <v>268</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1">
-        <v>290</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>290</v>
-      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>121</v>
+        <v>300</v>
       </c>
       <c r="D15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>242</v>
+        <f>SUM(C15*D15)</f>
+        <v>300</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>355</v>
+        <v>84</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>355</v>
+        <f>SUM(C16*D16)</f>
+        <v>252</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="8"/>
@@ -1453,43 +1458,62 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>134</v>
+        <f>SUM(C17*D17)</f>
+        <v>114</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>290</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f>SUM(C18*D18)</f>
+        <v>290</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1">
-        <v>41</v>
+        <v>121</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C19*D19)</f>
+        <v>242</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="8"/>
@@ -1497,123 +1521,105 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1">
-        <v>28</v>
+        <v>355</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C20*D20)</f>
+        <v>355</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f>SUM(C21*D21)</f>
+        <v>134</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="1">
-        <v>268</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>268</v>
-      </c>
+      <c r="A22" s="13"/>
       <c r="F22" s="5"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41</v>
+      </c>
+      <c r="E23">
+        <f>SUM(C23*D23)</f>
+        <v>0</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>41</v>
+      <c r="A24" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>SUM(C24*D24)</f>
+        <v>0</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1">
-        <v>52</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1">
-        <v>52</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="13"/>
       <c r="E27" s="1"/>
       <c r="F27" s="5"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="13"/>
       <c r="E28" s="15">
         <f>SUM(E2:E27)</f>
         <v>3019</v>
@@ -1623,83 +1629,79 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="13"/>
       <c r="E29" s="1"/>
       <c r="F29" s="5"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="E30" s="1"/>
       <c r="F30" s="5"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="E31" s="1"/>
       <c r="F31" s="5"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="13"/>
       <c r="E32" s="1"/>
       <c r="F32" s="10"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="13"/>
       <c r="E33" s="1"/>
       <c r="F33" s="5"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="13"/>
       <c r="E34" s="1"/>
       <c r="F34" s="5"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="13"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="13"/>
       <c r="E36" s="1"/>
       <c r="F36" s="5"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="13"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="13"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="13"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="13"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="13"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -1725,53 +1727,53 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="13"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+      <c r="A48" s="13"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="13"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="13"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="13"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="13"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+      <c r="A53" s="13"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="13"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -1798,25 +1800,25 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="LED MAX7219" xr:uid="{1E4A80B1-A1ED-4971-B110-C4D2EC9BDF2D}"/>
-    <hyperlink ref="B11" r:id="rId2" display="SCHRACK ROTARY SWITCH" xr:uid="{C4DF7C7D-DDB8-45BF-A437-6B583CFD7719}"/>
-    <hyperlink ref="B12" r:id="rId3" xr:uid="{2E93ED3C-C6C4-4DB8-9085-AB7DC46E1AB7}"/>
-    <hyperlink ref="B13" r:id="rId4" xr:uid="{E32D0610-4C22-4143-96D4-42FE9407CDB8}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{83F11D3E-8A8B-4FEB-B3D4-42A68E9E9355}"/>
+    <hyperlink ref="B15" r:id="rId2" display="SCHRACK ROTARY SWITCH" xr:uid="{C4DF7C7D-DDB8-45BF-A437-6B583CFD7719}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{2E93ED3C-C6C4-4DB8-9085-AB7DC46E1AB7}"/>
+    <hyperlink ref="B17" r:id="rId4" xr:uid="{E32D0610-4C22-4143-96D4-42FE9407CDB8}"/>
+    <hyperlink ref="B18" r:id="rId5" xr:uid="{83F11D3E-8A8B-4FEB-B3D4-42A68E9E9355}"/>
     <hyperlink ref="B3" r:id="rId6" display="2DIGIT 0.8IN" xr:uid="{580D8A90-A525-4103-80BC-86692308D035}"/>
     <hyperlink ref="B2" r:id="rId7" display="3DIGIT 0.8IN" xr:uid="{F3A0F711-4E3D-437D-B6B1-08FEB77FF404}"/>
-    <hyperlink ref="B20" r:id="rId8" xr:uid="{D00301B1-351D-4B39-A492-6C9989CEBCC0}"/>
-    <hyperlink ref="B19" r:id="rId9" xr:uid="{3CD4033C-9B3A-4318-9D64-ACE96F523159}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{C37A50F1-209C-4A5D-A411-0A456C588DD1}"/>
+    <hyperlink ref="B24" r:id="rId8" xr:uid="{D00301B1-351D-4B39-A492-6C9989CEBCC0}"/>
+    <hyperlink ref="B23" r:id="rId9" xr:uid="{3CD4033C-9B3A-4318-9D64-ACE96F523159}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{C37A50F1-209C-4A5D-A411-0A456C588DD1}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{C12FBC33-BE35-4D16-A3DE-C0D5DD8DAB8D}"/>
-    <hyperlink ref="B16" r:id="rId12" display="B/W DOUBLE SWITCH" xr:uid="{C90E987D-AD3A-4993-9BF7-652E256C06B3}"/>
+    <hyperlink ref="B20" r:id="rId12" display="B/W DOUBLE SWITCH" xr:uid="{C90E987D-AD3A-4993-9BF7-652E256C06B3}"/>
     <hyperlink ref="B7" r:id="rId13" display="SD CARD MODULE" xr:uid="{00BC3802-F8D1-45E4-9144-911623178974}"/>
     <hyperlink ref="B6" r:id="rId14" xr:uid="{074DFFA5-B78D-49EA-8698-C94E992C0CE2}"/>
-    <hyperlink ref="B5" r:id="rId15" location="relatedFiles" xr:uid="{115571BD-5AA3-42A8-A209-B76666A562D6}"/>
-    <hyperlink ref="B22" r:id="rId16" xr:uid="{D06EEAAB-F557-458E-A548-9BBAD34798FD}"/>
-    <hyperlink ref="B24" r:id="rId17" xr:uid="{487581BC-3942-40B1-9A68-4FCD1588123D}"/>
-    <hyperlink ref="B25" r:id="rId18" xr:uid="{721B5926-F035-438B-B5B6-1DA9415413DF}"/>
-    <hyperlink ref="B26" r:id="rId19" display="JUMPER WIRES STRAIGT" xr:uid="{AEFDAEF5-2992-43DD-8C63-EB43B385D8BA}"/>
-    <hyperlink ref="B17" r:id="rId20" xr:uid="{15437A6C-D298-45C0-863D-AE58A8E10838}"/>
+    <hyperlink ref="B5" r:id="rId15" location="relatedFiles" display="ESP32" xr:uid="{115571BD-5AA3-42A8-A209-B76666A562D6}"/>
+    <hyperlink ref="B13" r:id="rId16" display="DRIVER " xr:uid="{D06EEAAB-F557-458E-A548-9BBAD34798FD}"/>
+    <hyperlink ref="B10" r:id="rId17" display="JUMPER WIRES YURI" xr:uid="{487581BC-3942-40B1-9A68-4FCD1588123D}"/>
+    <hyperlink ref="B11" r:id="rId18" display="JUMPER WIRES YAOI" xr:uid="{721B5926-F035-438B-B5B6-1DA9415413DF}"/>
+    <hyperlink ref="B12" r:id="rId19" display="JUMPER WIRES STRAIGT" xr:uid="{AEFDAEF5-2992-43DD-8C63-EB43B385D8BA}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{15437A6C-D298-45C0-863D-AE58A8E10838}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>

</xml_diff>